<commit_message>
Fix code in atomic_piston
Refinamiento de métodos en:
1. atomic_piston
</commit_message>
<xml_diff>
--- a/atomic_piston/IPU/componentes_discretos.xlsx
+++ b/atomic_piston/IPU/componentes_discretos.xlsx
@@ -1,17 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gerardomayor/Documents/GitHub/watchers_refined/atomic_piston/IPU/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAAA3BD8-9D5E-C147-8B17-D9C74799C2A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="¡Gracias! Dame un listado de lo" sheetId="1" r:id="rId4"/>
+    <sheet name="¡Gracias! Dame un listado de lo" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'¡Gracias! Dame un listado de lo'!$A$1:$J$60</definedName>
+  </definedNames>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="74">
   <si>
     <t>Categoría</t>
   </si>
@@ -23,9 +35,6 @@
   </si>
   <si>
     <t>Notas Clave para la Cotización (Especificar con Proveedor)</t>
-  </si>
-  <si>
-    <t>Genera un presupuesto con las cantidades exactas...</t>
   </si>
   <si>
     <t>I. Microcontrolador y Periféricos Avanzados</t>
@@ -241,21 +250,40 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="d-m"/>
+    <numFmt numFmtId="164" formatCode="d\-m"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
     </font>
   </fonts>
   <fills count="2">
@@ -263,11 +291,17 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="10">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF284E3F"/>
@@ -281,6 +315,7 @@
       <bottom style="thin">
         <color rgb="FF284E3F"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -295,20 +330,7 @@
       <bottom style="thin">
         <color rgb="FF284E3F"/>
       </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF356854"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF284E3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF284E3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF284E3F"/>
-      </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -323,6 +345,7 @@
       <bottom style="thin">
         <color rgb="FFFFFFFF"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -337,6 +360,7 @@
       <bottom style="thin">
         <color rgb="FFFFFFFF"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -351,6 +375,7 @@
       <bottom style="thin">
         <color rgb="FFF6F8F9"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -365,6 +390,7 @@
       <bottom style="thin">
         <color rgb="FFF6F8F9"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -379,6 +405,7 @@
       <bottom style="thin">
         <color rgb="FF284E3F"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -393,120 +420,199 @@
       <bottom style="thin">
         <color rgb="FF284E3F"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="15">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="9">
     <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <border/>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Aptos"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font/>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Aptos"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Aptos"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF6F8F9"/>
+          <bgColor rgb="FFF6F8F9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FF356854"/>
           <bgColor rgb="FF356854"/>
         </patternFill>
       </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF6F8F9"/>
-          <bgColor rgb="FFF6F8F9"/>
-        </patternFill>
-      </fill>
-      <border/>
     </dxf>
   </dxfs>
   <tableStyles count="1">
-    <tableStyle count="3" pivot="0" name="¡Gracias! Dame un listado de lo-style">
-      <tableStyleElement dxfId="1" type="headerRow"/>
-      <tableStyleElement dxfId="2" type="firstRowStripe"/>
-      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+    <tableStyle name="¡Gracias! Dame un listado de lo-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+      <tableStyleElement type="headerRow" dxfId="8"/>
+      <tableStyleElement type="firstRowStripe" dxfId="7"/>
+      <tableStyleElement type="secondRowStripe" dxfId="6"/>
     </tableStyle>
   </tableStyles>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:E30" displayName="Tabla_1" name="Tabla_1" id="1">
-  <tableColumns count="5">
-    <tableColumn name="Categoría" id="1"/>
-    <tableColumn name="Componente Discreto" id="2"/>
-    <tableColumn name="Cantidad (Unidades)" id="3"/>
-    <tableColumn name="Notas Clave para la Cotización (Especificar con Proveedor)" id="4"/>
-    <tableColumn name="Genera un presupuesto con las cantidades exactas..." id="5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla_1" displayName="Tabla_1" ref="A1:C60" headerRowDxfId="5" dataDxfId="4" totalsRowDxfId="3">
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Categoría" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Componente Discreto" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Cantidad (Unidades)" dataDxfId="0"/>
   </tableColumns>
-  <tableStyleInfo name="¡Gracias! Dame un listado de lo-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <tableStyleInfo name="¡Gracias! Dame un listado de lo-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -696,28 +802,30 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A2" zoomScale="83" zoomScaleNormal="100" zoomScalePageLayoutView="83" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="2" width="37.63"/>
-    <col customWidth="1" min="3" max="3" width="20.75"/>
-    <col customWidth="1" min="4" max="5" width="37.63"/>
+    <col min="1" max="1" width="57.5" customWidth="1"/>
+    <col min="2" max="2" width="99.83203125" customWidth="1"/>
+    <col min="3" max="3" width="79" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -727,360 +835,503 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5"/>
+      <c r="B3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="5"/>
+      <c r="B4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="7">
+        <v>45718</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="5"/>
+      <c r="B5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="7">
+        <v>45749</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="5"/>
+      <c r="B7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="8">
+        <v>45749</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="5"/>
+      <c r="B8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="7">
+        <v>45749</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="5"/>
+      <c r="B9" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="8">
+        <v>45718</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="5"/>
+      <c r="B10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="7">
+        <v>45812</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="5"/>
+      <c r="B11" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="8">
+        <v>45718</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="5"/>
+      <c r="B12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="7">
+        <v>45718</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="5"/>
+      <c r="B14" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="7">
+        <v>45749</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="5"/>
+      <c r="B15" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="8">
+        <v>45689</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="7">
+        <v>45749</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="5"/>
+      <c r="B17" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="8">
+        <v>45873</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="5"/>
+      <c r="B19" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="5"/>
+      <c r="B20" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="7">
+        <v>45780</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="8">
+        <v>45718</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="5"/>
+      <c r="B22" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="8">
+        <v>45873</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="5"/>
+      <c r="B24" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="5"/>
+      <c r="B25" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="5"/>
+      <c r="B26" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="5"/>
+      <c r="B27" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="5"/>
+      <c r="B28" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="5"/>
+      <c r="B29" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="5"/>
+      <c r="B31" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="5" t="s">
+      <c r="C31" s="5"/>
+    </row>
+    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="5"/>
+      <c r="B32" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="B3" s="6" t="s">
+      <c r="C32" s="5"/>
+    </row>
+    <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="5"/>
+      <c r="B33" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="B4" s="5" t="s">
+      <c r="C33" s="5"/>
+    </row>
+    <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="5"/>
+      <c r="B34" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="7">
-        <v>45718.0</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" s="6" t="s">
+      <c r="C34" s="5"/>
+    </row>
+    <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="5"/>
+      <c r="B35" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="5" t="s">
+      <c r="C35" s="5"/>
+    </row>
+    <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="5"/>
+      <c r="B36" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="7">
-        <v>45749.0</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" s="6" t="s">
+      <c r="C36" s="5"/>
+    </row>
+    <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="5"/>
+      <c r="B37" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="8">
-        <v>45749.0</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="B8" s="5" t="s">
+      <c r="C37" s="5"/>
+    </row>
+    <row r="38" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="5"/>
+      <c r="B38" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="7">
-        <v>45749.0</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" s="6" t="s">
+      <c r="C38" s="5"/>
+    </row>
+    <row r="39" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="5"/>
+      <c r="B39" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="8">
-        <v>45718.0</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="B10" s="5" t="s">
+      <c r="C39" s="5"/>
+    </row>
+    <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="5"/>
+      <c r="B40" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="7">
-        <v>45812.0</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="B11" s="6" t="s">
+      <c r="C40" s="5"/>
+    </row>
+    <row r="41" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="5"/>
+      <c r="B41" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="8">
-        <v>45718.0</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="B12" s="5" t="s">
+      <c r="C41" s="5"/>
+    </row>
+    <row r="42" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="5"/>
+      <c r="B42" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="7">
-        <v>45718.0</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="6" t="s">
+      <c r="C42" s="5"/>
+    </row>
+    <row r="43" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="5"/>
+      <c r="B43" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="B14" s="5" t="s">
+      <c r="C43" s="5"/>
+    </row>
+    <row r="44" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="5"/>
+      <c r="B44" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="7">
-        <v>45749.0</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="B15" s="6" t="s">
+      <c r="C44" s="5"/>
+    </row>
+    <row r="45" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="5"/>
+      <c r="B45" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="8">
-        <v>45689.0</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" s="5" t="s">
+      <c r="C45" s="5"/>
+    </row>
+    <row r="46" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="5"/>
+      <c r="B46" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="7">
-        <v>45749.0</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="B17" s="6" t="s">
+      <c r="C46" s="5"/>
+    </row>
+    <row r="47" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="5"/>
+      <c r="B47" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="8">
-        <v>45873.0</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B18" s="5" t="s">
+      <c r="C47" s="5"/>
+    </row>
+    <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="5"/>
+      <c r="B48" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="5">
-        <v>2.0</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="B19" s="6" t="s">
+      <c r="C48" s="5"/>
+    </row>
+    <row r="49" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="5"/>
+      <c r="B49" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="B20" s="5" t="s">
+      <c r="C49" s="5"/>
+    </row>
+    <row r="50" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="5"/>
+      <c r="B50" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C20" s="7">
-        <v>45780.0</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B21" s="6" t="s">
+      <c r="C50" s="5"/>
+    </row>
+    <row r="51" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="5"/>
+      <c r="B51" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="8">
-        <v>45718.0</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="B22" s="5" t="s">
+      <c r="C51" s="5"/>
+    </row>
+    <row r="52" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="5"/>
+      <c r="B52" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C22" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="B23" s="6" t="s">
+      <c r="C52" s="5"/>
+    </row>
+    <row r="53" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="5"/>
+      <c r="B53" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="C23" s="8">
-        <v>45873.0</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="B24" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C24" s="5" t="s">
+      <c r="C53" s="5"/>
+    </row>
+    <row r="54" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="5"/>
+      <c r="B54" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D24" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="B25" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C25" s="6" t="s">
+      <c r="C54" s="5"/>
+    </row>
+    <row r="55" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="5"/>
+      <c r="B55" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="D25" s="6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="B26" s="5" t="s">
+      <c r="C55" s="5"/>
+    </row>
+    <row r="56" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="5"/>
+      <c r="B56" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C26" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="B27" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C27" s="6" t="s">
+      <c r="C56" s="5"/>
+    </row>
+    <row r="57" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="5"/>
+      <c r="B57" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="D27" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="B28" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C28" s="5" t="s">
+      <c r="C57" s="5"/>
+    </row>
+    <row r="58" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="5"/>
+      <c r="B58" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D28" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="B29" s="6" t="s">
+      <c r="C58" s="5"/>
+    </row>
+    <row r="59" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="5"/>
+      <c r="B59" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="C29" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="B30" s="11" t="s">
+      <c r="C59" s="5"/>
+    </row>
+    <row r="60" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="12"/>
+      <c r="B60" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="C30" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>74</v>
-      </c>
+      <c r="C60" s="12"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="51" pageOrder="overThenDown" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="3" max="59" man="1"/>
+  </colBreaks>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>